<commit_message>
More fire rule question
</commit_message>
<xml_diff>
--- a/Players/Kai/cost_value_hire.xlsx
+++ b/Players/Kai/cost_value_hire.xlsx
@@ -344,7 +344,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,29 +367,29 @@
   </sheetPr>
   <dimension ref="B2:Z24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="2.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="3.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15"/>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>3</v>
@@ -1207,11 +1207,11 @@
       </c>
       <c r="V16" s="0" t="n">
         <f aca="false">(SUM(E16:L16)+N16-7+M16+(R16/10))*O16</f>
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="W16" s="5" t="n">
         <f aca="false">V16/P16</f>
-        <v>0.633333333333333</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="X16" s="5" t="n">
         <v>0</v>

</xml_diff>